<commit_message>
Fixed bug in postprocessing and new Bosch use case
Former-commit-id: 3c2103a3bb52dabfafc8efb488ab2b9f00365d63
</commit_message>
<xml_diff>
--- a/data/adapter_sdm/flexis/Szenario1-84Sek_gut_mit_location.xlsx
+++ b/data/adapter_sdm/flexis/Szenario1-84Sek_gut_mit_location.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebas\OneDrive\Documents\prodsim\data\adapter_sdm\flexis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80903CC0-1329-4E27-AC8A-012615288199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B915D941-09DC-4D7B-A604-6280E696F801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="24940" windowHeight="15900" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ApplicationName" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">Capability!$A$1:$A$50</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8">Machine!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8">Machine!$A$1:$Q$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6">Order!$A$1:$K$129</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12">ProcessTime!$A$1:$C$85</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11">SetupTime!$A$1:$D$169</definedName>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2824" uniqueCount="799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2826" uniqueCount="801">
   <si>
     <t>name:String</t>
   </si>
@@ -2467,6 +2467,12 @@
   </si>
   <si>
     <t>SDM4FZI</t>
+  </si>
+  <si>
+    <t>x_location:int</t>
+  </si>
+  <si>
+    <t>y_location:int</t>
   </si>
 </sst>
 </file>
@@ -15708,7 +15714,9 @@
   </sheetPr>
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -15880,10 +15888,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15892,18 +15900,19 @@
     <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="35" style="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="35" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.54296875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="34.1796875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="36.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="35" style="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="35" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.54296875" style="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15917,35 +15926,41 @@
         <v>408</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="L1" s="22" t="s">
         <v>411</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="M1" s="22" t="s">
         <v>412</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>413</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="23"/>
-    </row>
-    <row r="2" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q1" s="23"/>
+    </row>
+    <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>414</v>
       </c>
@@ -15960,34 +15975,40 @@
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="3">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="3" t="str">
-        <f t="shared" ref="F2:F13" si="2">"~"&amp;LEFT(A2,FIND("_",A2)-1)&amp;"~"</f>
+      <c r="H2" s="3" t="str">
+        <f t="shared" ref="H2:H13" si="2">"~"&amp;LEFT(A2,FIND("_",A2)-1)&amp;"~"</f>
         <v>~Vorbereitung~</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="H2" s="3" t="str">
-        <f t="shared" ref="H2:H10" si="3">"Duration_"&amp;C2</f>
+      <c r="J2" s="3" t="str">
+        <f t="shared" ref="J2:J10" si="3">"Duration_"&amp;C2</f>
         <v>Duration_Vorbereitung</v>
       </c>
-      <c r="J2" s="24">
+      <c r="L2" s="24">
         <v>0</v>
       </c>
-      <c r="K2" s="24">
+      <c r="M2" s="24">
         <v>1</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>415</v>
       </c>
-      <c r="O2" s="24">
+      <c r="Q2" s="24">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>416</v>
       </c>
@@ -16002,34 +16023,40 @@
       <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="3">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="3" t="str">
+      <c r="H3" s="3" t="str">
         <f t="shared" si="2"/>
         <v>~Vorbereitung~</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="H3" s="3" t="str">
+      <c r="J3" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Duration_Vorbereitung</v>
       </c>
-      <c r="J3" s="24">
+      <c r="L3" s="24">
         <v>0</v>
       </c>
-      <c r="K3" s="24">
+      <c r="M3" s="24">
         <v>1</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>415</v>
       </c>
-      <c r="O3" s="24">
+      <c r="Q3" s="24">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>417</v>
       </c>
@@ -16044,34 +16071,40 @@
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="3">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="3" t="str">
+      <c r="H4" s="3" t="str">
         <f t="shared" si="2"/>
         <v>~Vormontage1~</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="H4" s="3" t="str">
+      <c r="J4" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Duration_Vormontage1</v>
       </c>
-      <c r="J4" s="24">
+      <c r="L4" s="24">
         <v>0</v>
       </c>
-      <c r="K4" s="24">
+      <c r="M4" s="24">
         <v>1</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>415</v>
       </c>
-      <c r="O4" s="24">
+      <c r="Q4" s="24">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>418</v>
       </c>
@@ -16086,34 +16119,40 @@
       <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="3">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="3" t="str">
+      <c r="H5" s="3" t="str">
         <f t="shared" si="2"/>
         <v>~Vormontage1~</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="H5" s="3" t="str">
+      <c r="J5" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Duration_Vormontage1</v>
       </c>
-      <c r="J5" s="24">
+      <c r="L5" s="24">
         <v>0</v>
       </c>
-      <c r="K5" s="24">
+      <c r="M5" s="24">
         <v>1</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>415</v>
       </c>
-      <c r="O5" s="24">
+      <c r="Q5" s="24">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>419</v>
       </c>
@@ -16128,34 +16167,40 @@
       <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="3">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3">
+        <v>25</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="3" t="str">
+      <c r="H6" s="3" t="str">
         <f t="shared" si="2"/>
         <v>~Vormontage2~</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="H6" s="3" t="str">
+      <c r="J6" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Duration_Vormontage2</v>
       </c>
-      <c r="J6" s="24">
+      <c r="L6" s="24">
         <v>0</v>
       </c>
-      <c r="K6" s="24">
+      <c r="M6" s="24">
         <v>1</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>415</v>
       </c>
-      <c r="O6" s="24">
+      <c r="Q6" s="24">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>420</v>
       </c>
@@ -16170,34 +16215,40 @@
       <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="3">
+        <v>30</v>
+      </c>
+      <c r="F7" s="3">
+        <v>30</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="3" t="str">
+      <c r="H7" s="3" t="str">
         <f t="shared" si="2"/>
         <v>~Vormontage2~</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="H7" s="3" t="str">
+      <c r="J7" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Duration_Vormontage2</v>
       </c>
-      <c r="J7" s="24">
+      <c r="L7" s="24">
         <v>0</v>
       </c>
-      <c r="K7" s="24">
+      <c r="M7" s="24">
         <v>1</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>415</v>
       </c>
-      <c r="O7" s="24">
+      <c r="Q7" s="24">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>421</v>
       </c>
@@ -16212,34 +16263,40 @@
       <c r="D8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="3">
+        <v>35</v>
+      </c>
+      <c r="F8" s="3">
+        <v>35</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="3" t="str">
+      <c r="H8" s="3" t="str">
         <f t="shared" si="2"/>
         <v>~Reinigung~</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="H8" s="3" t="str">
+      <c r="J8" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Duration_Reinigung</v>
       </c>
-      <c r="J8" s="24">
+      <c r="L8" s="24">
         <v>0</v>
       </c>
-      <c r="K8" s="24">
+      <c r="M8" s="24">
         <v>1</v>
       </c>
-      <c r="M8" t="s">
+      <c r="O8" t="s">
         <v>415</v>
       </c>
-      <c r="O8" s="24">
+      <c r="Q8" s="24">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>422</v>
       </c>
@@ -16254,34 +16311,40 @@
       <c r="D9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="3">
+        <v>40</v>
+      </c>
+      <c r="F9" s="3">
+        <v>40</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="3" t="str">
+      <c r="H9" s="3" t="str">
         <f t="shared" si="2"/>
         <v>~Reinigung~</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="H9" s="3" t="str">
+      <c r="J9" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Duration_Reinigung</v>
       </c>
-      <c r="J9" s="24">
+      <c r="L9" s="24">
         <v>0</v>
       </c>
-      <c r="K9" s="24">
+      <c r="M9" s="24">
         <v>1</v>
       </c>
-      <c r="M9" t="s">
+      <c r="O9" t="s">
         <v>415</v>
       </c>
-      <c r="O9" s="24">
+      <c r="Q9" s="24">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>423</v>
       </c>
@@ -16296,34 +16359,40 @@
       <c r="D10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="3">
+        <v>45</v>
+      </c>
+      <c r="F10" s="3">
+        <v>45</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="3" t="str">
+      <c r="H10" s="3" t="str">
         <f t="shared" si="2"/>
         <v>~SensordeckelMontage~</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="H10" s="3" t="str">
+      <c r="J10" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Duration_SensordeckelMontage</v>
       </c>
-      <c r="J10" s="24">
+      <c r="L10" s="24">
         <v>0</v>
       </c>
-      <c r="K10" s="24">
+      <c r="M10" s="24">
         <v>1</v>
       </c>
-      <c r="M10" t="s">
+      <c r="O10" t="s">
         <v>415</v>
       </c>
-      <c r="O10" s="24">
+      <c r="Q10" s="24">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>424</v>
       </c>
@@ -16338,33 +16407,39 @@
       <c r="D11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="3">
+        <v>50</v>
+      </c>
+      <c r="F11" s="3">
+        <v>50</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="3" t="str">
+      <c r="H11" s="3" t="str">
         <f t="shared" si="2"/>
         <v>~SchneckenradMontage~</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="J11" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="J11" s="24">
+      <c r="L11" s="24">
         <v>0</v>
       </c>
-      <c r="K11" s="24">
+      <c r="M11" s="24">
         <v>1</v>
       </c>
-      <c r="M11" t="s">
+      <c r="O11" t="s">
         <v>415</v>
       </c>
-      <c r="O11" s="24">
+      <c r="Q11" s="24">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>425</v>
       </c>
@@ -16379,33 +16454,39 @@
       <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="3">
+        <v>55</v>
+      </c>
+      <c r="F12" s="3">
+        <v>55</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="3" t="str">
+      <c r="H12" s="3" t="str">
         <f t="shared" si="2"/>
         <v>~SchneckenradMontage~</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="J12" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="J12" s="24">
+      <c r="L12" s="24">
         <v>0</v>
       </c>
-      <c r="K12" s="24">
+      <c r="M12" s="24">
         <v>1</v>
       </c>
-      <c r="M12" t="s">
+      <c r="O12" t="s">
         <v>415</v>
       </c>
-      <c r="O12" s="24">
+      <c r="Q12" s="24">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>426</v>
       </c>
@@ -16420,32 +16501,38 @@
       <c r="D13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="3">
+        <v>60</v>
+      </c>
+      <c r="F13" s="3">
+        <v>60</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="3" t="str">
+      <c r="H13" s="3" t="str">
         <f t="shared" si="2"/>
         <v>~Schmierung~</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3" t="str">
+      <c r="I13" s="3"/>
+      <c r="J13" s="3" t="str">
         <f>"Duration_"&amp;C13</f>
         <v>Duration_Schmierung</v>
       </c>
-      <c r="J13" s="24">
+      <c r="L13" s="24">
         <v>0</v>
       </c>
-      <c r="K13" s="24">
+      <c r="M13" s="24">
         <v>1</v>
       </c>
-      <c r="M13" t="s">
+      <c r="O13" t="s">
         <v>415</v>
       </c>
-      <c r="O13" s="24">
+      <c r="Q13" s="24">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -16453,11 +16540,13 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="O14" s="23"/>
-    </row>
-    <row r="15" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="Q14" s="23"/>
+    </row>
+    <row r="15" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -16465,9 +16554,11 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="O15" s="23"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="Q15" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>